<commit_message>
Revert "Add Column B"
This reverts commit 3e76292d064113b35323eb596fbc1e751754d54f.
</commit_message>
<xml_diff>
--- a/TestFile.xlsx
+++ b/TestFile.xlsx
@@ -21,26 +21,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -356,52 +336,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>